<commit_message>
Arbetstider dag 3 + user stories
Mer potentiella nya user stories
</commit_message>
<xml_diff>
--- a/Arbetstider.xlsx
+++ b/Arbetstider.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Arbetstider" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks och buggar" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Alexander</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Bugs fixed</t>
+  </si>
+  <si>
+    <t>Known bugs</t>
+  </si>
+  <si>
+    <t>Bugs left</t>
+  </si>
+  <si>
+    <t>Tasks done</t>
+  </si>
+  <si>
+    <t>Tasks</t>
   </si>
 </sst>
 </file>
@@ -602,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,9 +763,33 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
       <c r="L6">
         <f>SUM(C6:J6)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1053,39 +1092,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ref="C35:J35" si="0">SUM(C4:C32)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="L35" s="5">
         <f>SUM(L4:L32)</f>
-        <v>122</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1096,143 +1135,434 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>42</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2, -C2)</f>
+        <v>42</v>
+      </c>
+      <c r="E2" s="1">
         <v>41373</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(F2, -G2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <f>D2</f>
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f>SUM(B3, -C3)</f>
         <v>30</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>41374</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>SUM(F3, -G3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>D3</f>
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>SUM(B4, -C4)</f>
+        <v>26</v>
+      </c>
+      <c r="E4" s="1">
+        <v>41375</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <f>SUM(F4, -G4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>D4</f>
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <f>SUM(B5, -C5)</f>
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <f>SUM(F5, -G5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>D5</f>
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <f>SUM(B6, -C6)</f>
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <f>SUM(F6, -G6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>D6</f>
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <f>SUM(B7, -C7)</f>
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <f>SUM(F7, -G7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>D7</f>
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <f>SUM(B8, -C8)</f>
+        <v>26</v>
+      </c>
+      <c r="H8">
+        <f>SUM(F8, -G8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>D8</f>
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <f>SUM(B9, -C9)</f>
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <f>SUM(F9, -G9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>D9</f>
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <f>SUM(B10, -C10)</f>
+        <v>26</v>
+      </c>
+      <c r="H10">
+        <f>SUM(F10, -G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>D10</f>
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <f>SUM(B11, -C11)</f>
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <f>SUM(F11, -G11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>D11</f>
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <f>SUM(B12, -C12)</f>
+        <v>26</v>
+      </c>
+      <c r="H12">
+        <f>SUM(F12, -G12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>D12</f>
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <f>SUM(B13, -C13)</f>
+        <v>26</v>
+      </c>
+      <c r="H13">
+        <f>SUM(F13, -G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>D13</f>
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <f>SUM(B14, -C14)</f>
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <f>SUM(F14, -G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>D14</f>
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <f>SUM(B15, -C15)</f>
+        <v>26</v>
+      </c>
+      <c r="H15">
+        <f>SUM(F15, -G15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>D15</f>
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <f>SUM(B16, -C16)</f>
+        <v>26</v>
+      </c>
+      <c r="H16">
+        <f>SUM(F16, -G16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>D16</f>
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <f>SUM(B17, -C17)</f>
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <f>SUM(F17, -G17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>D17</f>
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <f>SUM(B18, -C18)</f>
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <f>SUM(F18, -G18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>D18</f>
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <f>SUM(B19, -C19)</f>
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <f>SUM(F19, -G19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>D19</f>
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <f>SUM(B20, -C20)</f>
+        <v>26</v>
+      </c>
+      <c r="H20">
+        <f>SUM(F20, -G20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>D20</f>
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <f>SUM(B21, -C21)</f>
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <f>SUM(F21, -G21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
+      </c>
+      <c r="B22">
+        <f>D21</f>
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <f>SUM(B22, -C22)</f>
+        <v>26</v>
+      </c>
+      <c r="H22">
+        <f>SUM(F22, -G22)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arbetstider dag 4, vecka 1 klar
Woop woop
</commit_message>
<xml_diff>
--- a/Arbetstider.xlsx
+++ b/Arbetstider.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" tabRatio="563" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arbetstider" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Alexander</t>
   </si>
@@ -171,16 +171,28 @@
     <t>Bugs fixed</t>
   </si>
   <si>
-    <t>Known bugs</t>
-  </si>
-  <si>
     <t>Bugs left</t>
   </si>
   <si>
     <t>Tasks done</t>
   </si>
   <si>
-    <t>Tasks</t>
+    <t>Total tasks</t>
+  </si>
+  <si>
+    <t>Tasks added</t>
+  </si>
+  <si>
+    <t>Bugs added</t>
+  </si>
+  <si>
+    <t>Total bugs</t>
+  </si>
+  <si>
+    <t>Total done</t>
+  </si>
+  <si>
+    <t>Total fixed</t>
   </si>
 </sst>
 </file>
@@ -617,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,9 +811,33 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
       <c r="L7">
         <f>SUM(C7:J7)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1092,39 +1128,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ref="C35:J35" si="0">SUM(C4:C32)</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L35" s="5">
         <f>SUM(L4:L32)</f>
-        <v>186</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1135,19 +1171,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1155,25 +1191,22 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1183,387 +1216,325 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>SUM(B2, -C2)</f>
-        <v>42</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" s="1">
         <v>41373</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>SUM(F2, -G2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f>D2</f>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
-      <c r="D3">
-        <f>SUM(B3, -C3)</f>
-        <v>30</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="1">
         <v>41374</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>SUM(F3, -G3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>D3</f>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4">
-        <f>SUM(B4, -C4)</f>
-        <v>26</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="1">
         <v>41375</v>
       </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <f>SUM(F4, -G4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <f>D4</f>
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <f>SUM(B5, -C5)</f>
-        <v>26</v>
-      </c>
-      <c r="H5">
-        <f>SUM(F5, -G5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41376</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <f>D5</f>
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <f>SUM(B6, -C6)</f>
-        <v>26</v>
-      </c>
-      <c r="H6">
-        <f>SUM(F6, -G6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>41379</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <f>D6</f>
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <f>SUM(B7, -C7)</f>
-        <v>26</v>
-      </c>
-      <c r="H7">
-        <f>SUM(F7, -G7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>41380</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <f>D7</f>
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <f>SUM(B8, -C8)</f>
-        <v>26</v>
-      </c>
-      <c r="H8">
-        <f>SUM(F8, -G8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>41381</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <f>D8</f>
-        <v>26</v>
-      </c>
-      <c r="D9">
-        <f>SUM(B9, -C9)</f>
-        <v>26</v>
-      </c>
-      <c r="H9">
-        <f>SUM(F9, -G9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>41382</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <f>D9</f>
-        <v>26</v>
-      </c>
-      <c r="D10">
-        <f>SUM(B10, -C10)</f>
-        <v>26</v>
-      </c>
-      <c r="H10">
-        <f>SUM(F10, -G10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>41383</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f>D10</f>
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <f>SUM(B11, -C11)</f>
-        <v>26</v>
-      </c>
-      <c r="H11">
-        <f>SUM(F11, -G11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>41386</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <f>D11</f>
-        <v>26</v>
-      </c>
-      <c r="D12">
-        <f>SUM(B12, -C12)</f>
-        <v>26</v>
-      </c>
-      <c r="H12">
-        <f>SUM(F12, -G12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>41387</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <f>D12</f>
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <f>SUM(B13, -C13)</f>
-        <v>26</v>
-      </c>
-      <c r="H13">
-        <f>SUM(F13, -G13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>41388</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <f>D13</f>
-        <v>26</v>
-      </c>
-      <c r="D14">
-        <f>SUM(B14, -C14)</f>
-        <v>26</v>
-      </c>
-      <c r="H14">
-        <f>SUM(F14, -G14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>41389</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <f>D14</f>
-        <v>26</v>
-      </c>
-      <c r="D15">
-        <f>SUM(B15, -C15)</f>
-        <v>26</v>
-      </c>
-      <c r="H15">
-        <f>SUM(F15, -G15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>41390</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <f>D15</f>
-        <v>26</v>
-      </c>
-      <c r="D16">
-        <f>SUM(B16, -C16)</f>
-        <v>26</v>
-      </c>
-      <c r="H16">
-        <f>SUM(F16, -G16)</f>
-        <v>0</v>
+      <c r="D16" s="1">
+        <v>41393</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <f>D16</f>
-        <v>26</v>
-      </c>
-      <c r="D17">
-        <f>SUM(B17, -C17)</f>
-        <v>26</v>
-      </c>
-      <c r="H17">
-        <f>SUM(F17, -G17)</f>
-        <v>0</v>
+      <c r="D17" s="1">
+        <v>41394</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <f>D17</f>
-        <v>26</v>
-      </c>
-      <c r="D18">
-        <f>SUM(B18, -C18)</f>
-        <v>26</v>
-      </c>
-      <c r="H18">
-        <f>SUM(F18, -G18)</f>
-        <v>0</v>
+      <c r="D18" s="1">
+        <v>41396</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <f>D18</f>
-        <v>26</v>
-      </c>
-      <c r="D19">
-        <f>SUM(B19, -C19)</f>
-        <v>26</v>
-      </c>
-      <c r="H19">
-        <f>SUM(F19, -G19)</f>
-        <v>0</v>
+      <c r="D19" s="1">
+        <v>41397</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <f>D19</f>
-        <v>26</v>
-      </c>
-      <c r="D20">
-        <f>SUM(B20, -C20)</f>
-        <v>26</v>
-      </c>
-      <c r="H20">
-        <f>SUM(F20, -G20)</f>
-        <v>0</v>
+      <c r="D20" s="1">
+        <v>41400</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <f>D20</f>
-        <v>26</v>
-      </c>
-      <c r="D21">
-        <f>SUM(B21, -C21)</f>
-        <v>26</v>
-      </c>
-      <c r="H21">
-        <f>SUM(F21, -G21)</f>
-        <v>0</v>
+      <c r="D21" s="1">
+        <v>41401</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <f>D21</f>
-        <v>26</v>
-      </c>
-      <c r="D22">
-        <f>SUM(B22, -C22)</f>
-        <v>26</v>
-      </c>
-      <c r="H22">
-        <f>SUM(F22, -G22)</f>
-        <v>0</v>
-      </c>
+      <c r="D22" s="1">
+        <v>41402</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B2:B22)</f>
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24">
+        <f>SUM(C2:C22)</f>
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24">
+        <f>SUM(B24, -E24)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <f>SUM(E2:E22)</f>
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25">
+        <f>SUM(F2:F22)</f>
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25">
+        <f>SUM(B25, -E25)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixade arbetstiderna igen lawl (dag 4)
</commit_message>
<xml_diff>
--- a/Arbetstider.xlsx
+++ b/Arbetstider.xlsx
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>41376</v>
@@ -1498,14 +1498,14 @@
       </c>
       <c r="E24">
         <f>SUM(C2:C22)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
         <v>47</v>
       </c>
       <c r="H24">
         <f>SUM(B24, -E24)</f>
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Arbetstider dag 5 + PRGRS RPRT
Tja
</commit_message>
<xml_diff>
--- a/Arbetstider.xlsx
+++ b/Arbetstider.xlsx
@@ -9,14 +9,17 @@
   <sheets>
     <sheet name="Arbetstider" sheetId="1" r:id="rId1"/>
     <sheet name="Tasks och buggar" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Progress it.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Progress it.2" sheetId="4" r:id="rId4"/>
+    <sheet name="Progress it.3" sheetId="5" r:id="rId5"/>
+    <sheet name="Progress it.4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="103">
   <si>
     <t>Alexander</t>
   </si>
@@ -193,6 +196,218 @@
   </si>
   <si>
     <t>Total fixed</t>
+  </si>
+  <si>
+    <t>Grupp</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>olo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upp</t>
+    </r>
+  </si>
+  <si>
+    <t>Estimaterad tid</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DHD</t>
+    </r>
+  </si>
+  <si>
+    <t>Anslut över LAN</t>
+  </si>
+  <si>
+    <t>Specifiera Port</t>
+  </si>
+  <si>
+    <t>Specifiera IP</t>
+  </si>
+  <si>
+    <t>Fixat socket från Android</t>
+  </si>
+  <si>
+    <t>Skicka int till server</t>
+  </si>
+  <si>
+    <t>Disconnect-knapp</t>
+  </si>
+  <si>
+    <t>Skicka Δx Δy</t>
+  </si>
+  <si>
+    <t>Server GUI</t>
+  </si>
+  <si>
+    <t>4 dagar (32 timmar)</t>
+  </si>
+  <si>
+    <t>Connect socket</t>
+  </si>
+  <si>
+    <t>Skicka input till robot handler</t>
+  </si>
+  <si>
+    <t>Visa lokal IP</t>
+  </si>
+  <si>
+    <t>Visa global IP</t>
+  </si>
+  <si>
+    <t>Bestämma port</t>
+  </si>
+  <si>
+    <t>Känna klient DC, stanna uppe</t>
+  </si>
+  <si>
+    <t>Kunna disconnecta</t>
+  </si>
+  <si>
+    <t>Re-connect</t>
+  </si>
+  <si>
+    <t>App GUI</t>
+  </si>
+  <si>
+    <t>Tid (timmar)</t>
+  </si>
+  <si>
+    <t>Få fram tangentbordet</t>
+  </si>
+  <si>
+    <t>Läs av rörelse</t>
+  </si>
+  <si>
+    <t>Räkna ut Δx Δy</t>
+  </si>
+  <si>
+    <t>Läs av knapptryck</t>
+  </si>
+  <si>
+    <t>Macro GUI</t>
+  </si>
+  <si>
+    <t>Macros</t>
+  </si>
+  <si>
+    <t>Default macros</t>
+  </si>
+  <si>
+    <t>Skicka macros</t>
+  </si>
+  <si>
+    <t>Testa macros</t>
+  </si>
+  <si>
+    <t>Testa mus</t>
+  </si>
+  <si>
+    <t>6 dagar (48 timmar)</t>
+  </si>
+  <si>
+    <t>Simulera musklick</t>
+  </si>
+  <si>
+    <t>Ta skärmdump</t>
+  </si>
+  <si>
+    <t>Simulera knapptryck</t>
+  </si>
+  <si>
+    <t>Ta emot chars</t>
+  </si>
+  <si>
+    <t>Ta emot och hantera mus</t>
+  </si>
+  <si>
+    <t>Ta emot macros</t>
+  </si>
+  <si>
+    <t>2 dagar (16 timmar)</t>
   </si>
 </sst>
 </file>
@@ -258,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -307,6 +522,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -315,13 +579,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -630,7 +906,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,9 +1142,33 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
       <c r="L10">
         <f>SUM(C10:J10)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,39 +1428,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ref="C35:J35" si="0">SUM(C4:C32)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L35" s="5">
         <f>SUM(L4:L32)</f>
-        <v>250</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -1174,7 +1474,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,8 +1602,20 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6" s="1">
         <v>41379</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1491,7 +1803,7 @@
       </c>
       <c r="B24">
         <f>SUM(B2:B22)</f>
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>57</v>
@@ -1505,7 +1817,7 @@
       </c>
       <c r="H24">
         <f>SUM(B24, -E24)</f>
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1514,14 +1826,14 @@
       </c>
       <c r="B25">
         <f>SUM(E2:E22)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
         <v>58</v>
       </c>
       <c r="E25">
         <f>SUM(F2:F22)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
         <v>51</v>
@@ -1543,12 +1855,1570 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12">
+        <f>SUM(C2:C8)</f>
+        <v>10.5</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
+        <f>SUM(C10:C18)</f>
+        <v>14</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="8">
+        <v>4</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="12">
+        <f>SUM(C20:C30)</f>
+        <v>15.5</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="8">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="8">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C32:C37)</f>
+        <v>9.5</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="B32:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
+        <f>SUM(C10:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="12">
+        <f>SUM(C20:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C32:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
+        <f>SUM(C10:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="12">
+        <f>SUM(C20:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C32:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="E15:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
+        <f>SUM(C10:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="12">
+        <f>SUM(C20:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C32:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>